<commit_message>
fix:update the gradio demo's examples
</commit_message>
<xml_diff>
--- a/gradio_demo/模型演示.xlsx
+++ b/gradio_demo/模型演示.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16640" activeTab="2"/>
+    <workbookView windowWidth="27660" windowHeight="13040" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="对话" sheetId="4" r:id="rId1"/>
@@ -82,47 +82,55 @@
     <t>北京市道路运输条例第十八条</t>
   </si>
   <si>
-    <t>冷却系统为什么不能添加自来水</t>
-  </si>
-  <si>
-    <t>如往冷却系统添加自来水，冷却系统内部会堆积水垢，当温度在零度以下时，会产生结冰，并且严重影响冷却系统工作。市面上销售的瓶装防冻剂都添加了防锈、腐剂。当它稀释时，将失去抗锈、腐能力。防冻剂的稀释浓度必须与制造商说明的一致。给冷却系统添加冷却液时，它的颜色是绿色并且含乙二醇。当环境温度在-35℃时，请选用冰点低于-35℃的冷却液。
-98冷却液检查冷却液检查在水平地面上使用边撑撑起车辆；扶正车辆并检查副水箱冷却液液位；如果冷却液水平面位于 A 区域：排出多余冷却液至 B 区域；如果冷却液水平面位于 B 区域：液位合适；如果冷却液水平面位于 C 区域或不可见：补充相同冷却液至B 区域。警告警告冷却液在车辆行驶时温度会非常高，并处于受压状态。在发动机或冷却系统彻底冷却前，不可打开散热器、散热器软管、副水箱等其他任何冷却系统零部件。一旦发生烫伤，使用流动冷水冲洗伤口 10 分钟以上至伤口不再疼痛后及时就医。冷却液添加冷却液添加打开副水箱盖并添加相同的冷却液至 B 区域。警示警示如果需要经常补充冷却液，或副水箱内的冷却液经常被倒吸干，可能冷却系统出现泄露，联系您的经销商检查冷却系统。仅推荐使用春风动力原厂冷却液，不同的冷却液混合后可能造成发动机损坏，联系您的经销商更换冷却液</t>
-  </si>
-  <si>
-    <t>250SR使用说明书片段</t>
-  </si>
-  <si>
-    <t>有人说，开车走过很多遍的道路，如果骑着摩托车再去会看到截然不同的景色。
-《禅与摩托车维修艺术》一书中也写过：“坐在汽车里，你只是被局限在一个小空间之内，因为已经习惯了，你意识不到从车窗向外看风景和看电视差不多。你只个被动的观众，景物只能呆板地从窗外飞驰而过。骑摩托车可就不同了。它没有什么车窗玻璃在面前阻挡你视野，你会感到自己和大自然紧密地结合在了一起。你就处在景致之中，而不再是观众，你能感受到那种身临其境的震撼。”</t>
-  </si>
-  <si>
-    <t>摩托车专题报告片段</t>
-  </si>
-  <si>
-    <t>一箱啤酒出现几个玻璃厂生产的酒瓶混合使用的情况，应该是真的还是假冒品牌？</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-瓶盖的真假主要从油墨的印刷质量来鉴别。青岛啤酒瓶盖主要有蓝色、红色、绿色、棕紫色、灰色、黑色，蓝色用于内销酒，红色用于出口酒、金标酒，绿色用于出口酒，棕紫色用于棕色啤酒，灰色用于淡啤酒，黑色用于黑啤酒。
-青岛啤酒所使用的瓶盖视觉清晰、细腻、光滑，盖面“青岛啤酒”字样与栈桥图形、英文字母清楚，瓶盖裙边的“青岛啤酒”小字样非常清晰，瓶盖内是PVC模压胶垫，内有字码，胶垫与瓶盖不易分离。
-假冒青啤瓶盖，油墨印刷质量粗糙、歪斜，盖面油墨印刷直观感觉不好，颜色暗淡不正，瓶盖裙边的“青岛啤酒”字样模糊不清，有的假冒盖裙边没有这四个字，手感不润滑，瓶盖胶垫有的是橡胶垫，有的是滴塑垫，很容易使其与瓶盖分离。
-青岛啤酒有限公司为确保产品质量，所生产的“青岛”牌啤酒全部采用新瓶子主要供瓶厂家有“青岛晶华玻璃厂，青岛玻璃厂，崂山玻璃厂，胶州市玻璃厂，青岛北海玻璃厂，南定玻璃厂”，这些厂家用都属山东省日用玻璃行业。一箱啤酒一般不会出现几个玻璃厂生产的酒瓶混合使用的情况。假冒青啤（640ml）使用的瓶子，用回收的旧瓶，什么厂家生产的都有，也有可能上述几种瓶子混合使用。如果出现该公司从没使用的瓶子，一看便可确认是假冒。</t>
+    <t>参观须知</t>
+  </si>
+  <si>
+    <t xml:space="preserve">北京故宫博物院，成立于1925年10月10日。是在明清皇宫及其收藏基础上建立起来的集古代建筑群、宫廷收藏、历代文化艺术为一体的大型综合性博物馆。 也是中国最大的古代文化艺术博物馆。 
+北京故宫博物院占地100余万平方米，保存古建筑约9000间，是中国现存规模最大、保存最完整的古代宫殿建筑群。故宫的前身是明清皇宫紫禁城，于明永乐十八年（1420年）建成，明清两代共有24位皇帝居住于此。1912年溥仪退位后，紫禁城作为皇宫的历史就此终结。1914年，于外朝区域成立古物陈列所；1925年，于内廷区域成立故宫博物院；1948年，古物陈列所并入故宫博物院。 
+北京故宫博物院院藏文物体系完备，现有藏品总量180万余件（套），藏品总分25种大类别，其中一级藏品8000余件（套）。 依据不同质地和形式，可分为绘画、法书、碑帖、铜器、金银器等25大类，其中珍贵文物占藏品总数的90%。故宫博物院通过明清皇家宫殿建筑，宫廷史迹原状陈列，珍宝、钟表、书画、陶瓷、雕塑等艺术藏品常设展览， 每年还定期举办临时专题展览。 
+参观须知：
+1.尊重文化遗产，保护文物古迹：请不要在古建筑和古树上留下您的大名，刻画涂写不仅不会使您英名永驻，反而遭到大家的鄙视。
+2.做文明观众：不妨碍、影响他人参观，按照国际惯例在展厅请勿使用闪光灯和三脚架拍照。在我院与其他博物馆合作举办的展览以及特色商品店，因有版权协议，不允许观众拍照展品，请注意警示标志并服从展厅工作人员的管理。
+3.文明环境靠大家共同营造：请勿携带宠物进院参观。请尽量不妨碍其他观众。请保持衣容整洁。不要做出有碍观瞻、有损形象的行为。为了您和他人的健康，请勿随地吐痰。请勿乱丢垃圾废物请您尊重清洁工人的劳动。让我们共同保持参观环境的清洁有序！
+</t>
+  </si>
+  <si>
+    <t>故宫片段</t>
+  </si>
+  <si>
+    <t>猎户星空（Orion Star）创⽴于 2016 年9⽉，是由猎豹移动投资的智能服务机器⼈公司。 猎户星空为“真有⽤”机器⼈⽽⽣，以“让⼈们从重复的体⼒劳动中解放出来，让传统商业像互联⽹⼀样⾼效”为愿景，成为“智能+”时代的中国服务机器⼈新物种公司
+猎户星空在⾏业内率先提出“AI+软件+硬件+服务=机器⼈”的公式。基于这⼀公式，独家打造了⾏业唯⼀⾃研全链条AI技术，拥有机器⼈操作系统应⽤开发能⼒、全栈硬件设计制造能⼒、全国⽹点服务能⼒。</t>
+  </si>
+  <si>
+    <t>猎户星空片段</t>
+  </si>
+  <si>
+    <t>青岛啤酒酒精含量是多少？</t>
+  </si>
+  <si>
+    <t xml:space="preserve">山西老陈醋是中国四大名醋之一，已有3000余年的历史，素有“天下第一醋”的盛誉，以色、香、醇、浓、酸五大特征著称于世。 山西老陈醋色泽呈酱红色，食之绵、酸、香、甜、鲜。 山西老陈醋含有丰富的氨基酸、有机酸、糖类、维生素和盐等。以老陈醋为基质的保健醋有软化血管、降低甘油三酯等独特功效。
+山西老陈醋是以高粱、麸皮、谷糠和水为主要原料，以大麦、豌豆所制大曲为糖化发酵剂，经酒精发酵后，再经固态醋酸发酵、熏醅、陈酿等工序酿制而成。其主要酿造工艺特点为：以高粱为主的多种原料配比，以红心大曲为主的优质糖化发酵剂，低温浓醪酒精发酵，高温固态醋酸发酵，熏醅和新醋长期陈酿。
+曲质优良
+微生物种丰富：其它名优食醋使用的小曲主要是根霉和酵母，麦曲主要是黄曲霉，红曲主要是红曲霉，上述微生物种群在红心大曲中都能体现，而红心大曲中的其它微生物种群在上述曲种未必都能得到体现，特别是大曲中含有丰富的霉素，使山西老陈醋形成特有的香气和气味。
+熏醅技术
+源于山西，熏香味是山西食醋的典型风味：熏醅是山西食醋的独特技艺，可使山西老陈醋的酯香、熏香、陈香有机复合；同时熏醅也可获得山西老陈醋的满意色泽，与其它名优食醋相比，不需外加调色剂。
+突出陈酿
+以新醋陈酿代替簇醅陈酿：镇江香醋、四川保宁麸醋等均为醋醅陈酿代替新醋陈酿，陈酿期分别为20—30天和一年左右；唯有山西老陈醋是以新醋陈酿代替醋醅陈酿，陈酿期一般为9—12个月，有的长达数年之久。传统工艺称为“夏伏晒，冬捞冰”，新醋经日晒蒸发和冬捞冰后，其浓缩倍数达3倍以上。山西老陈醋总酸在9～11度，其比重、浓度、粘稠度、可溶性固形物以及不挥发酸、总糖、还原糖、总酯、氨基酸态氮等质量指标，均可名列全国食醋之首。并由于陈酿过程中酯酸转化，醇醛缩合，不挥发酸比例增加，使老陈醋陈香细腻，酸味柔和。
+</t>
+  </si>
+  <si>
+    <t>山西老陈醋片段</t>
+  </si>
+  <si>
+    <t>青岛啤酒产自青岛啤酒股份有限公司，公司的前身是国营青岛啤酒厂，1903年由英、德两国商人合资开办，是最早的啤酒生产企业之一。2008年北京奥运会官方赞助商，跻身世界品牌500强。
+青岛啤酒选用优质大麦、大米、上等啤酒花和软硬适度、洁净甘美的崂山矿泉水为原料酿制而成。原麦汁浓度为十二度，酒精含量3.5－4%。酒液清澈透明、呈淡黄色，泡沫清白、细腻而持久。
+2018年12月18日，世界品牌实验室发布《2018世界品牌500强》，青岛啤酒排名第310。
+2019年4月10日，青岛啤酒第41届“提高质量纪念日”主题活动——“匠心筑梦，开创魅力质量新时代”在青岛啤酒二厂举行 。
+2019年12月，青岛啤酒入选2019中国品牌强国盛典榜样100品牌。
+2019年12月18日，人民日报“中国品牌发展指数”100榜单排名第91位。</t>
   </si>
   <si>
     <t>青岛啤酒片段</t>
-  </si>
-  <si>
-    <t>山西老陈醋是中国四大名醋之一，它的生产已有 3000 年余年的历史，全山西大大小小
-的醋生产企业也有 1000 多家。号称中国四大名醋之一的山西老陈醋以其绵、酸、香、甜、
-醇的独特风味和悠久的酿造历史熏在国内排名位居镇江醋、保宁醋和福建红曲醋之前，著称
-于世。已故著名微生物学家方心芳先生，早在 20 世纪 30 年代就对“美和居”山西老陈醋的
-工艺进行了总结和肯定，他在《黄海》杂志上发表文章指出：“清源醋之发酵温度高至 40℃
-以上，其酪酸菌、乳酸菌必起作用，山西醋之气味别致足可证明醋酸菌以外的细菌作用。”
-并称：“我国有四大名醋，首推山西老陈醋”。已故著名生物学家陈驹声先生则在多种著作
-中明确指出：“山西老陈醋是我国北方最著名的食醋”。</t>
-  </si>
-  <si>
-    <t>山西陈醋片段</t>
   </si>
   <si>
     <t>序号</t>
@@ -1339,10 +1347,10 @@
   <sheetPr/>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.234375" defaultRowHeight="16.8" outlineLevelRow="6" outlineLevelCol="2"/>
@@ -1385,7 +1393,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" ht="252" spans="1:3">
+    <row r="4" ht="409.5" spans="1:3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1407,7 +1415,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" ht="286" spans="1:3">
+    <row r="6" ht="409.5" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -1440,7 +1448,7 @@
   <sheetPr/>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>

</xml_diff>